<commit_message>
Updated assert library to testng assert
</commit_message>
<xml_diff>
--- a/Testdata.xlsx
+++ b/Testdata.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>FirstName</t>
   </si>
@@ -50,25 +50,46 @@
     <t>Password</t>
   </si>
   <si>
-    <t>4547###</t>
-  </si>
-  <si>
     <t>Company BBB</t>
   </si>
   <si>
-    <t>Tom</t>
-  </si>
-  <si>
-    <t>matt</t>
-  </si>
-  <si>
-    <t>Blue</t>
-  </si>
-  <si>
-    <t>matt@comp.com</t>
-  </si>
-  <si>
-    <t>111222333</t>
+    <t>Pass1</t>
+  </si>
+  <si>
+    <t>Company AAA</t>
+  </si>
+  <si>
+    <t>admin@mail.com</t>
+  </si>
+  <si>
+    <t>082555</t>
+  </si>
+  <si>
+    <t>083444</t>
+  </si>
+  <si>
+    <t>cusomter@mail.com</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>LName1</t>
+  </si>
+  <si>
+    <t>User1</t>
+  </si>
+  <si>
+    <t>User2</t>
+  </si>
+  <si>
+    <t>LName2</t>
+  </si>
+  <si>
+    <t>FName2</t>
+  </si>
+  <si>
+    <t>FName1</t>
   </si>
 </sst>
 </file>
@@ -398,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,35 +465,62 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" t="s">
         <v>8</v>
-      </c>
-      <c r="H2" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>